<commit_message>
Se corrige template excel y el modelo del reporte
</commit_message>
<xml_diff>
--- a/inc/templates/templateNew.xlsx
+++ b/inc/templates/templateNew.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>GESTIÓN ADMINISTRATIVA</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>Observaciones</t>
-  </si>
-  <si>
-    <t>ATENCIÓN DE SOLICITUDES ASOCIADOS A ORDENES DE TRABAJO</t>
   </si>
 </sst>
 </file>
@@ -277,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -364,23 +361,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -425,16 +411,10 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -450,63 +430,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -804,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
-      <selection activeCell="BV8" sqref="BV8"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BJ13" sqref="BJ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -822,118 +792,119 @@
     <col min="10" max="10" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.42578125" style="2" customWidth="1"/>
-    <col min="13" max="55" width="5.7109375" style="2" customWidth="1"/>
-    <col min="56" max="80" width="3.7109375" style="2" customWidth="1"/>
+    <col min="13" max="61" width="5.7109375" style="2" customWidth="1"/>
+    <col min="62" max="62" width="29.140625" style="2" customWidth="1"/>
+    <col min="63" max="80" width="3.7109375" style="2" customWidth="1"/>
     <col min="81" max="86" width="5.7109375" style="2" customWidth="1"/>
-    <col min="87" max="87" width="70.7109375" style="2" customWidth="1"/>
+    <col min="87" max="87" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="88" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:87" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="34" t="s">
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="38" t="s">
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="34" t="s">
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="38" t="s">
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="34" t="s">
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="33" t="s">
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
-      <c r="AO1" s="33"/>
-      <c r="AP1" s="34" t="s">
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="39" t="s">
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="AU1" s="40"/>
-      <c r="AV1" s="40"/>
-      <c r="AW1" s="40"/>
-      <c r="AX1" s="40"/>
-      <c r="AY1" s="40"/>
-      <c r="AZ1" s="40"/>
-      <c r="BA1" s="40"/>
-      <c r="BB1" s="40"/>
-      <c r="BC1" s="40"/>
-      <c r="BD1" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="BE1" s="30"/>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30"/>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
-      <c r="BM1" s="30"/>
-      <c r="BN1" s="30"/>
-      <c r="BO1" s="30"/>
-      <c r="BP1" s="30"/>
-      <c r="BQ1" s="30"/>
-      <c r="BR1" s="30"/>
-      <c r="BS1" s="30"/>
-      <c r="BT1" s="30"/>
-      <c r="BU1" s="30"/>
-      <c r="BV1" s="30"/>
-      <c r="BW1" s="30"/>
-      <c r="BX1" s="30"/>
-      <c r="BY1" s="30"/>
-      <c r="BZ1" s="30"/>
-      <c r="CA1" s="30"/>
-      <c r="CB1" s="31"/>
-      <c r="CC1" s="32" t="s">
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="CD1" s="32"/>
-      <c r="CE1" s="32"/>
-      <c r="CF1" s="32"/>
-      <c r="CG1" s="32"/>
-      <c r="CH1" s="21" t="s">
+      <c r="BE1" s="33"/>
+      <c r="BF1" s="33"/>
+      <c r="BG1" s="33"/>
+      <c r="BH1" s="33"/>
+      <c r="BI1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="CI1" s="22"/>
+      <c r="BJ1" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="BK1"/>
+      <c r="BL1"/>
+      <c r="BM1"/>
+      <c r="BN1"/>
+      <c r="BO1"/>
+      <c r="BP1"/>
+      <c r="BQ1"/>
+      <c r="BR1"/>
+      <c r="BS1"/>
+      <c r="BT1"/>
+      <c r="BU1"/>
+      <c r="BV1"/>
+      <c r="BW1"/>
+      <c r="BX1"/>
+      <c r="BY1"/>
+      <c r="BZ1"/>
+      <c r="CA1"/>
+      <c r="CB1"/>
+      <c r="CC1"/>
+      <c r="CD1"/>
+      <c r="CE1"/>
+      <c r="CF1"/>
+      <c r="CG1"/>
+      <c r="CH1"/>
+      <c r="CI1" s="20"/>
     </row>
-    <row r="2" spans="1:87" ht="153.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:87" ht="153.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1099,67 +1070,67 @@
       <c r="BC2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="BD2" s="23"/>
-      <c r="BE2" s="23"/>
-      <c r="BF2" s="23"/>
-      <c r="BG2" s="23"/>
-      <c r="BH2" s="23"/>
-      <c r="BI2" s="23"/>
-      <c r="BJ2" s="23"/>
-      <c r="BK2" s="23"/>
-      <c r="BL2" s="23"/>
-      <c r="BM2" s="23"/>
-      <c r="BN2" s="23"/>
-      <c r="BO2" s="23"/>
-      <c r="BP2" s="23"/>
-      <c r="BQ2" s="23"/>
-      <c r="BR2" s="23"/>
-      <c r="BS2" s="23"/>
-      <c r="BT2" s="23"/>
-      <c r="BU2" s="23"/>
-      <c r="BV2" s="23"/>
-      <c r="BW2" s="23"/>
-      <c r="BX2" s="23"/>
-      <c r="BY2" s="23"/>
-      <c r="BZ2" s="23"/>
-      <c r="CA2" s="23"/>
-      <c r="CB2" s="23"/>
-      <c r="CC2" s="26" t="s">
+      <c r="BD2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="CD2" s="26" t="s">
+      <c r="BE2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="CE2" s="26" t="s">
+      <c r="BF2" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="CF2" s="26" t="s">
+      <c r="BG2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="CG2" s="26" t="s">
+      <c r="BH2" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="CH2" s="29" t="s">
+      <c r="BI2" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="CI2" s="24" t="s">
+      <c r="BJ2" s="34" t="s">
         <v>44</v>
       </c>
+      <c r="BK2"/>
+      <c r="BL2"/>
+      <c r="BM2"/>
+      <c r="BN2"/>
+      <c r="BO2"/>
+      <c r="BP2"/>
+      <c r="BQ2"/>
+      <c r="BR2"/>
+      <c r="BS2"/>
+      <c r="BT2"/>
+      <c r="BU2"/>
+      <c r="BV2"/>
+      <c r="BW2"/>
+      <c r="BX2"/>
+      <c r="BY2"/>
+      <c r="BZ2"/>
+      <c r="CA2"/>
+      <c r="CB2"/>
+      <c r="CC2"/>
+      <c r="CD2"/>
+      <c r="CE2"/>
+      <c r="CF2"/>
+      <c r="CG2"/>
+      <c r="CH2"/>
+      <c r="CI2"/>
     </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="16"/>
+    <row r="3" spans="1:87" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="15"/>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
@@ -1202,43 +1173,43 @@
       <c r="BA3" s="14"/>
       <c r="BB3" s="14"/>
       <c r="BC3" s="14"/>
-      <c r="BD3" s="28"/>
-      <c r="BE3" s="28"/>
-      <c r="BF3" s="28"/>
-      <c r="BG3" s="28"/>
-      <c r="BH3" s="28"/>
-      <c r="BI3" s="28"/>
-      <c r="BJ3" s="15"/>
-      <c r="BK3" s="17"/>
-      <c r="BL3" s="25"/>
-      <c r="BM3" s="25"/>
-      <c r="BN3" s="25"/>
-      <c r="BO3" s="25"/>
-      <c r="BP3" s="25"/>
-      <c r="BQ3" s="25"/>
-      <c r="BR3" s="25"/>
-      <c r="BS3" s="25"/>
-      <c r="BT3" s="25"/>
-      <c r="BU3" s="25"/>
-      <c r="BV3" s="25"/>
-      <c r="BW3" s="25"/>
-      <c r="BX3" s="25"/>
-      <c r="BY3" s="25"/>
-      <c r="BZ3" s="25"/>
-      <c r="CA3" s="25"/>
-      <c r="CB3" s="25"/>
-      <c r="CC3" s="27"/>
-      <c r="CD3" s="27"/>
-      <c r="CE3" s="27"/>
-      <c r="CF3" s="27"/>
-      <c r="CG3" s="27"/>
-      <c r="CH3" s="25"/>
-      <c r="CI3" s="25"/>
+      <c r="BD3" s="22"/>
+      <c r="BE3" s="22"/>
+      <c r="BF3" s="22"/>
+      <c r="BG3" s="22"/>
+      <c r="BH3" s="22"/>
+      <c r="BI3" s="22"/>
+      <c r="BJ3"/>
+      <c r="BK3"/>
+      <c r="BL3"/>
+      <c r="BM3"/>
+      <c r="BN3"/>
+      <c r="BO3"/>
+      <c r="BP3"/>
+      <c r="BQ3"/>
+      <c r="BR3"/>
+      <c r="BS3"/>
+      <c r="BT3"/>
+      <c r="BU3"/>
+      <c r="BV3"/>
+      <c r="BW3"/>
+      <c r="BX3"/>
+      <c r="BY3"/>
+      <c r="BZ3"/>
+      <c r="CA3"/>
+      <c r="CB3"/>
+      <c r="CC3"/>
+      <c r="CD3"/>
+      <c r="CE3"/>
+      <c r="CF3"/>
+      <c r="CG3"/>
+      <c r="CH3"/>
+      <c r="CI3"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="BD1:CB1"/>
-    <mergeCell ref="CC1:CG1"/>
+  <mergeCells count="10">
+    <mergeCell ref="AT1:BC1"/>
+    <mergeCell ref="BD1:BH1"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="N1:Q1"/>
@@ -1247,7 +1218,6 @@
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AT1:BC1"/>
   </mergeCells>
   <conditionalFormatting sqref="BJ3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>